<commit_message>
Locators updated, select item and scrolling functionality added
Updated files:
 EbayMobileAutomation/src/test/java/ebaydemo/AddToCart.java
EbayMobileAutomation/src/main/java/com/pageObjects/EbayPageObject.java
EbayMobileAutomation/pom.xml
EbayMobileAutomation/tesData.xlsx
</commit_message>
<xml_diff>
--- a/EbayMobileAutomation/tesData.xlsx
+++ b/EbayMobileAutomation/tesData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E607C91E-8F08-433E-88BC-32F89E0A0CEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3B4169-1831-4F69-BD03-A39895A52B0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,19 +43,19 @@
     <t>description</t>
   </si>
   <si>
-    <t>65 inch tv</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
-    <t>700$</t>
-  </si>
-  <si>
     <t>TC_01</t>
   </si>
   <si>
     <t>modelNo</t>
+  </si>
+  <si>
+    <t>Samsung UN65NU6900FXZA 65 inch 2160p LED Smart TV</t>
+  </si>
+  <si>
+    <t>579.99$</t>
   </si>
 </sst>
 </file>
@@ -413,11 +413,12 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -438,21 +439,21 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>

</xml_diff>